<commit_message>
excelw: replaced test fixture
</commit_message>
<xml_diff>
--- a/cli/output/excelw/testdata/miscdb_tbl_types.xlsx
+++ b/cli/output/excelw/testdata/miscdb_tbl_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>col_id</t>
   </si>
@@ -76,9 +76,6 @@
     <t/>
   </si>
   <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>c2V2ZW4=</t>
-  </si>
-  <si>
-    <t>07:07:07</t>
   </si>
   <si>
     <t>77.77</t>
@@ -530,17 +524,17 @@
       <c r="O2" s="3">
         <v>32821</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -566,16 +560,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="2">
         <v>42923.2966087963</v>
@@ -589,17 +583,17 @@
       <c r="O3" s="3">
         <v>42923</v>
       </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>24</v>
+      <c r="P3" s="4">
+        <v>0.2966087962995516</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0.2966087962995516</v>
       </c>
       <c r="R3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -616,10 +610,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
       </c>
       <c r="L4" s="2">
         <v>42923.2966087963</v>
@@ -627,11 +621,11 @@
       <c r="N4" s="3">
         <v>42923</v>
       </c>
-      <c r="P4" t="s">
-        <v>24</v>
+      <c r="P4" s="4">
+        <v>0.2966087962995516</v>
       </c>
       <c r="R4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#200: Excel date format config (#294)
* Config options to control Excel date/time output format
</commit_message>
<xml_diff>
--- a/cli/output/excelw/testdata/miscdb_tbl_types.xlsx
+++ b/cli/output/excelw/testdata/miscdb_tbl_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>col_id</t>
   </si>
@@ -76,9 +76,6 @@
     <t/>
   </si>
   <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>c2V2ZW4=</t>
-  </si>
-  <si>
-    <t>07:07:07</t>
   </si>
   <si>
     <t>77.77</t>
@@ -530,17 +524,17 @@
       <c r="O2" s="3">
         <v>32821</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -566,16 +560,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="2">
         <v>42923.2966087963</v>
@@ -589,17 +583,17 @@
       <c r="O3" s="3">
         <v>42923</v>
       </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>24</v>
+      <c r="P3" s="4">
+        <v>0.2966087962995516</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0.2966087962995516</v>
       </c>
       <c r="R3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="S3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -616,10 +610,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
       </c>
       <c r="L4" s="2">
         <v>42923.2966087963</v>
@@ -627,11 +621,11 @@
       <c r="N4" s="3">
         <v>42923</v>
       </c>
-      <c r="P4" t="s">
-        <v>24</v>
+      <c r="P4" s="4">
+        <v>0.2966087962995516</v>
       </c>
       <c r="R4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>